<commit_message>
Added step-by-step guide, fixed Pinmap error
</commit_message>
<xml_diff>
--- a/docs/Pinmap.xlsx
+++ b/docs/Pinmap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3e342190b4c8ac1/Dokumente/Elektronik/Projekte/Tang9k_baseboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3e342190b4c8ac1/Dokumente/Elektronik/Projekte/t9k-baseboard/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="8_{BE1094FC-6705-4F72-BAF7-531673D1D3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B11F4ADA-573F-4806-9891-3AB065625EF4}"/>
+  <xr:revisionPtr revIDLastSave="204" documentId="8_{BE1094FC-6705-4F72-BAF7-531673D1D3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63DB2980-9AA2-4B69-B4FD-65EF71AC234E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{A1B50231-39FB-4493-BFDF-E9BEE12643D3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="104">
   <si>
     <t>Tang Nano 9k FPGA Base board</t>
   </si>
@@ -342,13 +342,19 @@
   </si>
   <si>
     <t>Note: All Buttons, Joysticks, Encoders or non-RGB LEDs are "Active-Low"!</t>
+  </si>
+  <si>
+    <t>1.8V</t>
+  </si>
+  <si>
+    <t>3.3V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +384,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -387,7 +401,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="60">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -408,15 +422,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1159,7 +1164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1177,6 +1182,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1186,69 +1194,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1267,7 +1272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1276,7 +1281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1288,95 +1293,98 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1720,7 +1728,7 @@
   <dimension ref="B1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1738,23 +1746,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="15">
+      <c r="B1" s="14">
         <v>45473</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="73" t="s">
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="52" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>100</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -1763,233 +1771,245 @@
       <c r="D2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="61"/>
+      <c r="F2" s="60"/>
       <c r="G2" s="6" t="s">
         <v>98</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="57"/>
-      <c r="G3" s="53" t="s">
+      <c r="C3" s="56"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="54"/>
-      <c r="I3" s="55"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="57"/>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="31">
+      <c r="B4" s="30">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="36">
         <v>39</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="72" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="12">
         <v>28</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="25">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="32">
+      <c r="B5" s="31">
         <v>1.2</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="8">
         <v>36</v>
       </c>
-      <c r="E5" s="59"/>
+      <c r="E5" s="73"/>
       <c r="F5" s="3"/>
       <c r="G5" s="7">
         <v>27</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="17">
         <v>1.2</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="32">
+      <c r="B6" s="31">
         <v>1.3</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="34" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="8">
         <v>37</v>
       </c>
-      <c r="E6" s="59"/>
+      <c r="E6" s="73"/>
       <c r="F6" s="3"/>
       <c r="G6" s="7">
         <v>26</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="17">
         <v>1.3</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <v>1.4</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="34" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="8">
         <v>38</v>
       </c>
-      <c r="E7" s="60"/>
+      <c r="E7" s="74"/>
       <c r="F7" s="3"/>
       <c r="G7" s="7">
         <v>25</v>
       </c>
-      <c r="H7" s="42" t="s">
+      <c r="H7" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="17">
         <v>1.4</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <v>1.5</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="34" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="8">
         <v>49</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="72" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="7">
         <v>34</v>
       </c>
-      <c r="H8" s="42" t="s">
+      <c r="H8" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="17">
         <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="32">
+      <c r="B9" s="31">
         <v>1.6</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="34" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="8">
         <v>48</v>
       </c>
-      <c r="E9" s="59"/>
+      <c r="E9" s="73"/>
       <c r="F9" s="3"/>
       <c r="G9" s="7">
         <v>33</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="H9" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="17">
         <v>1.6</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="32">
+      <c r="B10" s="31">
         <v>1.7</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="34" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="8">
         <v>76</v>
       </c>
-      <c r="E10" s="59"/>
+      <c r="E10" s="73"/>
       <c r="F10" s="3"/>
       <c r="G10" s="7">
         <v>30</v>
       </c>
-      <c r="H10" s="42" t="s">
+      <c r="H10" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="17">
         <v>1.7</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="33">
+      <c r="B11" s="32">
         <v>1.8</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="35" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="10">
         <v>77</v>
       </c>
-      <c r="E11" s="60"/>
+      <c r="E11" s="74"/>
       <c r="F11" s="3"/>
       <c r="G11" s="9">
         <v>29</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="20">
         <v>1.8</v>
       </c>
     </row>
     <row r="12" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="25"/>
-      <c r="I12" s="22"/>
+      <c r="B12" s="24"/>
+      <c r="I12" s="21"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="57"/>
-      <c r="G13" s="53" t="s">
+      <c r="C13" s="56"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="F13" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="54"/>
-      <c r="I13" s="55"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="57"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="19">
+      <c r="B14" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="37" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="11">
@@ -1998,18 +2018,18 @@
       <c r="G14" s="12">
         <v>32</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H14" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="25">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="20">
+      <c r="B15" s="19">
         <v>1.2</v>
       </c>
-      <c r="C15" s="39" t="s">
+      <c r="C15" s="38" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="8">
@@ -2018,18 +2038,18 @@
       <c r="G15" s="7">
         <v>31</v>
       </c>
-      <c r="H15" s="42" t="s">
+      <c r="H15" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="17">
         <v>1.2</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="20">
+      <c r="B16" s="19">
         <v>1.3</v>
       </c>
-      <c r="C16" s="39" t="s">
+      <c r="C16" s="38" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="8">
@@ -2038,18 +2058,18 @@
       <c r="G16" s="7">
         <v>57</v>
       </c>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="17">
         <v>1.3</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="20">
+      <c r="B17" s="19">
         <v>1.4</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="38" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="8">
@@ -2058,67 +2078,67 @@
       <c r="G17" s="9">
         <v>56</v>
       </c>
-      <c r="H17" s="43" t="s">
+      <c r="H17" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="20">
         <v>1.4</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="20">
+      <c r="B18" s="19">
         <v>1.5</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="38" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="8">
         <v>55</v>
       </c>
-      <c r="I18" s="22"/>
+      <c r="I18" s="21"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="20">
+      <c r="B19" s="19">
         <v>1.6</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="38" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="8">
         <v>54</v>
       </c>
-      <c r="G19" s="53" t="s">
+      <c r="G19" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="H19" s="54"/>
-      <c r="I19" s="55"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="57"/>
     </row>
     <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="20">
+      <c r="B20" s="19">
         <v>1.7</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="8">
         <v>53</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="45">
+      <c r="G20" s="44">
         <v>63</v>
       </c>
-      <c r="H20" s="44" t="s">
+      <c r="H20" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="22" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="24">
+      <c r="B21" s="23">
         <v>1.8</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="39" t="s">
         <v>35</v>
       </c>
       <c r="D21" s="10">
@@ -2126,37 +2146,43 @@
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="I21" s="22"/>
+      <c r="I21" s="21"/>
     </row>
     <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="25"/>
-      <c r="G22" s="53" t="s">
+      <c r="B22" s="24"/>
+      <c r="F22" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="H22" s="54"/>
-      <c r="I22" s="55"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="57"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="57"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="53" t="s">
+        <v>102</v>
+      </c>
       <c r="G23" s="12">
         <v>83</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="I23" s="26" t="s">
+      <c r="I23" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="37" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="11">
@@ -2165,18 +2191,18 @@
       <c r="G24" s="7">
         <v>82</v>
       </c>
-      <c r="H24" s="42" t="s">
+      <c r="H24" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="I24" s="17" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="38" t="s">
         <v>44</v>
       </c>
       <c r="D25" s="8">
@@ -2185,18 +2211,18 @@
       <c r="G25" s="7">
         <v>81</v>
       </c>
-      <c r="H25" s="42" t="s">
+      <c r="H25" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="I25" s="18" t="s">
+      <c r="I25" s="17" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="39" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="10">
@@ -2205,145 +2231,151 @@
       <c r="G26" s="7">
         <v>80</v>
       </c>
-      <c r="H26" s="42" t="s">
+      <c r="H26" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="I26" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="25"/>
+      <c r="B27" s="24"/>
       <c r="G27" s="9">
         <v>79</v>
       </c>
-      <c r="H27" s="43" t="s">
+      <c r="H27" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="I27" s="21" t="s">
+      <c r="I27" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="57"/>
-      <c r="I28" s="22"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="I28" s="21"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="37">
+      <c r="D29" s="36">
         <v>10</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="G29" s="53" t="s">
+      <c r="F29" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="H29" s="54"/>
-      <c r="I29" s="55"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="57"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="38" t="s">
         <v>64</v>
       </c>
       <c r="D30" s="8">
         <v>11</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="67" t="s">
+      <c r="F30" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="G30" s="46">
+      <c r="G30" s="45">
         <v>49</v>
       </c>
-      <c r="H30" s="41" t="s">
+      <c r="H30" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="26" t="s">
+      <c r="I30" s="25" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C31" s="38" t="s">
         <v>65</v>
       </c>
       <c r="D31" s="8">
         <v>13</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="47">
+      <c r="F31" s="67"/>
+      <c r="G31" s="46">
         <v>77</v>
       </c>
-      <c r="H31" s="42" t="s">
+      <c r="H31" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="I31" s="18" t="s">
+      <c r="I31" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="39" t="s">
+      <c r="C32" s="38" t="s">
         <v>66</v>
       </c>
       <c r="D32" s="8">
         <v>14</v>
       </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="47">
+      <c r="F32" s="67"/>
+      <c r="G32" s="46">
         <v>76</v>
       </c>
-      <c r="H32" s="42" t="s">
+      <c r="H32" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="18" t="s">
+      <c r="I32" s="17" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="39" t="s">
+      <c r="C33" s="38" t="s">
         <v>67</v>
       </c>
       <c r="D33" s="8">
         <v>15</v>
       </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="47">
+      <c r="F33" s="68"/>
+      <c r="G33" s="46">
         <v>48</v>
       </c>
-      <c r="H33" s="42" t="s">
+      <c r="H33" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="I33" s="18" t="s">
+      <c r="I33" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="39" t="s">
         <v>68</v>
       </c>
       <c r="D34" s="10">
@@ -2351,141 +2383,153 @@
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="49">
+      <c r="G34" s="48">
         <v>47</v>
       </c>
-      <c r="H34" s="43" t="s">
+      <c r="H34" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="I34" s="21" t="s">
+      <c r="I34" s="20" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="25"/>
-      <c r="I35" s="48"/>
+      <c r="B35" s="24"/>
+      <c r="I35" s="47"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="57"/>
-      <c r="G36" s="53" t="s">
+      <c r="C36" s="56"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="G36" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="54"/>
-      <c r="I36" s="55"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="57"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C37" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="36">
+        <v>4</v>
+      </c>
+      <c r="F37" s="69" t="s">
+        <v>75</v>
+      </c>
+      <c r="G37" s="45">
+        <v>38</v>
+      </c>
+      <c r="H37" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="37">
+      <c r="D38" s="10">
         <v>3</v>
       </c>
-      <c r="F37" s="70" t="s">
-        <v>75</v>
-      </c>
-      <c r="G37" s="46">
-        <v>38</v>
-      </c>
-      <c r="H37" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="10">
-        <v>4</v>
-      </c>
-      <c r="F38" s="71"/>
-      <c r="G38" s="47">
+      <c r="F38" s="70"/>
+      <c r="G38" s="46">
         <v>37</v>
       </c>
-      <c r="H38" s="42" t="s">
+      <c r="H38" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I38" s="18" t="s">
+      <c r="I38" s="17" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="39" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="25"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="47">
+      <c r="B39" s="24"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="46">
         <v>36</v>
       </c>
-      <c r="H39" s="42" t="s">
+      <c r="H39" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="I39" s="18" t="s">
+      <c r="I39" s="17" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="40" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="57"/>
-      <c r="F40" s="72"/>
-      <c r="G40" s="49">
+      <c r="C40" s="56"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="F40" s="71"/>
+      <c r="G40" s="48">
         <v>39</v>
       </c>
-      <c r="H40" s="43" t="s">
+      <c r="H40" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="I40" s="21" t="s">
+      <c r="I40" s="20" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="41" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="38" t="s">
+      <c r="C41" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="37">
+      <c r="D41" s="36">
         <v>61</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="I41" s="22"/>
+      <c r="I41" s="21"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="38" t="s">
         <v>83</v>
       </c>
       <c r="D42" s="8">
         <v>62</v>
       </c>
-      <c r="G42" s="53" t="s">
+      <c r="F42" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="G42" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="H42" s="54"/>
-      <c r="I42" s="55"/>
+      <c r="H42" s="56"/>
+      <c r="I42" s="57"/>
     </row>
     <row r="43" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="38" t="s">
         <v>84</v>
       </c>
       <c r="D43" s="8">
@@ -2494,68 +2538,70 @@
       <c r="G43" s="13">
         <v>52</v>
       </c>
-      <c r="H43" s="50" t="s">
+      <c r="H43" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="I43" s="27" t="s">
+      <c r="I43" s="26" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="24" t="s">
+      <c r="B44" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="40" t="s">
+      <c r="C44" s="39" t="s">
         <v>85</v>
       </c>
       <c r="D44" s="10">
         <v>60</v>
       </c>
-      <c r="I44" s="22"/>
+      <c r="I44" s="21"/>
     </row>
     <row r="45" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="62" t="s">
+      <c r="B45" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="53" t="s">
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="G45" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H45" s="54"/>
-      <c r="I45" s="55"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="57"/>
     </row>
     <row r="46" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="62"/>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="46">
+      <c r="B46" s="61"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="45">
         <v>17</v>
       </c>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="I46" s="26" t="s">
+      <c r="I46" s="25" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="47" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="64"/>
-      <c r="C47" s="65"/>
-      <c r="D47" s="65"/>
-      <c r="E47" s="65"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="52">
+      <c r="B47" s="63"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="51">
         <v>18</v>
       </c>
-      <c r="H47" s="51" t="s">
+      <c r="H47" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="I47" s="29" t="s">
+      <c r="I47" s="28" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>